<commit_message>
Smart Pass Success Rate added to the radar | Radar Scale Fixed
</commit_message>
<xml_diff>
--- a/draft.xlsx
+++ b/draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMMATION\PYTHON_PROJECTS\SoccerAnalytics_2017-2018_PremierLeague_WestHam_DefendersReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E99127-0BA2-464C-A610-F3CDB993D98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3B2BF8-CC30-49E0-BE6E-B0EADCF15235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14910" yWindow="285" windowWidth="13860" windowHeight="14430" xr2:uid="{84AD5316-8B25-4019-9A5E-947BAB871352}"/>
   </bookViews>
@@ -563,7 +563,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Conceded Goal Maps Fixed | Vitor Hugo Radar done
</commit_message>
<xml_diff>
--- a/draft.xlsx
+++ b/draft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMMATION\PYTHON_PROJECTS\SoccerAnalytics_2017-2018_PremierLeague_WestHam_DefendersReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3B2BF8-CC30-49E0-BE6E-B0EADCF15235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7389FFBC-9631-4848-9B8A-95154E8B3509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14910" yWindow="285" windowWidth="13860" windowHeight="14430" xr2:uid="{84AD5316-8B25-4019-9A5E-947BAB871352}"/>
+    <workbookView xWindow="1470" yWindow="720" windowWidth="19695" windowHeight="14430" xr2:uid="{84AD5316-8B25-4019-9A5E-947BAB871352}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>Match Played</t>
   </si>
@@ -165,6 +165,24 @@
   </si>
   <si>
     <t>Lopez</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>United</t>
+  </si>
+  <si>
+    <t>Tottenham</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>WestHam</t>
   </si>
 </sst>
 </file>
@@ -560,16 +578,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82B55FCA-A68F-42C7-880F-020476E9AC4F}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B14" sqref="B14:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -871,6 +889,60 @@
         <v>26</v>
       </c>
     </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14">
+        <f>8+5+5+3+1+1+1+1</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15">
+        <f>11+10+2+1+1+1</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16">
+        <f>13+7+5+4+2+1+1+1+1</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17">
+        <f>14+10+4+3+2+1+1</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18">
+        <f>11+10+6+3+3+2+1+1+1</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19">
+        <f>26+18+5+5+3+2+2+2+2+1</f>
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>